<commit_message>
Aggiunta tabella delle frequenze delle operazioni
</commit_message>
<xml_diff>
--- a/Relazione/Tabelle/TabellaVolumi.xlsx
+++ b/Relazione/Tabelle/TabellaVolumi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Desktop\Basi_Di_Dati_2021\Relazione\Tabelle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7432595-334D-4A21-8C0F-9F2E40309EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E5A8D7-7CB0-4FE8-AA40-33C60B95F6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{6FADB2D5-140B-46BE-9A40-7CF2C5F8C85D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FADB2D5-140B-46BE-9A40-7CF2C5F8C85D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,6 +315,7 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,7 +325,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -639,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2261ECB6-8C75-4385-AB02-C0BA08C27FE1}">
-  <dimension ref="B2:G31"/>
+  <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -650,18 +650,18 @@
     <col min="2" max="2" width="23.234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.5">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.5">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
@@ -672,7 +672,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
@@ -683,7 +683,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -693,8 +693,9 @@
       <c r="D6" s="13">
         <v>10000</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
@@ -705,7 +706,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
@@ -717,7 +718,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
@@ -728,7 +729,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B10" s="5" t="s">
         <v>10</v>
       </c>
@@ -739,7 +740,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
@@ -750,7 +751,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
@@ -761,7 +762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
@@ -772,7 +773,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -783,7 +784,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
@@ -794,7 +795,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.5">
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -969,7 +970,7 @@
       <c r="D31" s="13">
         <v>1000000</v>
       </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>